<commit_message>
Excel validations and question's creation
</commit_message>
<xml_diff>
--- a/resources/Data Injection.xlsx
+++ b/resources/Data Injection.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Contra12</t>
   </si>
@@ -40,12 +40,6 @@
     <t>Juan12345</t>
   </si>
   <si>
-    <t>ORDER PAYMENT</t>
-  </si>
-  <si>
-    <t>HP ENVY - 17T TOUCH LAPTO</t>
-  </si>
-  <si>
     <t xml:space="preserve">Daniel Miranda </t>
   </si>
   <si>
@@ -56,13 +50,25 @@
   </si>
   <si>
     <t>Carrera 56 # 50</t>
+  </si>
+  <si>
+    <t>Name:Daniel Miranda</t>
+  </si>
+  <si>
+    <t>Email:daniel@gmail.com</t>
+  </si>
+  <si>
+    <t>Current Address :Medellin calle 50</t>
+  </si>
+  <si>
+    <t>Permananet Address :Carrera 56 # 50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +92,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -108,11 +120,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -435,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,16 +468,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -474,25 +493,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>